<commit_message>
Features upd & dataset column corr.
</commit_message>
<xml_diff>
--- a/migforecasting/features.xlsx
+++ b/migforecasting/features.xlsx
@@ -54,58 +54,58 @@
     <t>Торговля</t>
   </si>
   <si>
-    <t xml:space="preserve">Численность населения 4 </t>
-  </si>
-  <si>
-    <t>Сред. численность работников 15</t>
-  </si>
-  <si>
-    <t>Безработные 17</t>
-  </si>
-  <si>
-    <t>Сред. з/п 19</t>
-  </si>
-  <si>
-    <t>Площадь на одного 22</t>
-  </si>
-  <si>
-    <t>Число дошкольных мест 23</t>
-  </si>
-  <si>
-    <t>Врачей на 10000 27</t>
-  </si>
-  <si>
-    <t>Число коек на 10000 34</t>
-  </si>
-  <si>
-    <t>Мощность поликлиник на 10000 38</t>
-  </si>
-  <si>
-    <t>Удельный вес 45</t>
-  </si>
-  <si>
-    <t>Степень износа 52</t>
-  </si>
-  <si>
-    <t>Число предприятий 55</t>
-  </si>
-  <si>
-    <t>Сумма четырех пунктов 58-61</t>
-  </si>
-  <si>
-    <t>объем работ 63</t>
-  </si>
-  <si>
-    <t>Ввод в действие жилых 64</t>
-  </si>
-  <si>
-    <t>Число постр. квартир 65</t>
-  </si>
-  <si>
-    <t>Оборот розницы 72</t>
-  </si>
-  <si>
-    <t>Оборот общепита 74</t>
+    <t>Численность населения - popsize (тыс)</t>
+  </si>
+  <si>
+    <t>Безработные - unemployed (шт)</t>
+  </si>
+  <si>
+    <t>Сред. Числ. работников - avgemployers (тыс)</t>
+  </si>
+  <si>
+    <t>Сред. з/п - avgsalary (руб)</t>
+  </si>
+  <si>
+    <t>Площадь на одного - livarea (м2)</t>
+  </si>
+  <si>
+    <t>Число дошкол. мест - beforeschool (тыс)</t>
+  </si>
+  <si>
+    <t>Врачей на 10000 - docsperpop (на 10 тыс)</t>
+  </si>
+  <si>
+    <t>Удельный вес - invests ( %)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Мощность поликлиник на 10000 - cliniccap </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Число коек на 10000 - bedsperpop </t>
+  </si>
+  <si>
+    <t>Степень износа -  funds %</t>
+  </si>
+  <si>
+    <t>Число предприятий - companies (шт)</t>
+  </si>
+  <si>
+    <t>Сумма четырех пунктов - factoriescap (сумма млн. руб.)</t>
+  </si>
+  <si>
+    <t>объем работ - conscap (млн. руб.)</t>
+  </si>
+  <si>
+    <t>Ввод в действие жилых - consnewareas (тыс. м2)</t>
+  </si>
+  <si>
+    <t>Число постр. квартир - consnewapt (шт)</t>
+  </si>
+  <si>
+    <t>Оборот розницы - retailturnover (млн. руб.)</t>
+  </si>
+  <si>
+    <t>Оборот общепита - foodservturnover (млн. руб)</t>
   </si>
 </sst>
 </file>
@@ -685,18 +685,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+      <selection activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="25.140625" customWidth="1"/>
-    <col min="2" max="2" width="26.5703125" customWidth="1"/>
-    <col min="3" max="3" width="32.85546875" customWidth="1"/>
-    <col min="4" max="4" width="35.7109375" customWidth="1"/>
-    <col min="5" max="5" width="29.140625" customWidth="1"/>
-    <col min="6" max="6" width="26.28515625" customWidth="1"/>
+    <col min="2" max="2" width="42.140625" customWidth="1"/>
+    <col min="3" max="3" width="57.42578125" customWidth="1"/>
+    <col min="4" max="4" width="54.140625" customWidth="1"/>
+    <col min="5" max="5" width="50.7109375" customWidth="1"/>
+    <col min="6" max="6" width="45.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.140625" customWidth="1"/>
     <col min="8" max="8" width="10.85546875" customWidth="1"/>
   </cols>
@@ -726,20 +726,20 @@
         <v>11</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D2" s="2" t="s">
         <v>14</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="2"/>
       <c r="C3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D3" s="2" t="s">
         <v>15</v>
@@ -769,7 +769,7 @@
       <c r="B6" s="2"/>
       <c r="C6" s="6"/>
       <c r="D6" s="2" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="E6" s="2"/>
     </row>

</xml_diff>

<commit_message>
Northwestern fed. dist. 10-11 (added)
</commit_message>
<xml_diff>
--- a/migforecasting/features.xlsx
+++ b/migforecasting/features.xlsx
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Dir. for small cities and Boks. area (part)
</commit_message>
<xml_diff>
--- a/migforecasting/features.xlsx
+++ b/migforecasting/features.xlsx
@@ -54,9 +54,6 @@
     <t>Торговля</t>
   </si>
   <si>
-    <t>Численность населения - popsize (тыс)</t>
-  </si>
-  <si>
     <t>Безработные - unemployed (шт)</t>
   </si>
   <si>
@@ -106,6 +103,9 @@
   </si>
   <si>
     <t>Инвест. в основной капитал / числ. населения - invest</t>
+  </si>
+  <si>
+    <t>Численность населения - popsize (тыс. чел.)</t>
   </si>
 </sst>
 </file>
@@ -685,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F4" sqref="F4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -723,26 +723,26 @@
         <v>3</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="C2" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="E2" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
       <c r="B3" s="2"/>
       <c r="C3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="E3" s="2"/>
     </row>
@@ -751,7 +751,7 @@
       <c r="B4" s="2"/>
       <c r="C4" s="6"/>
       <c r="D4" s="2" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E4" s="2"/>
     </row>
@@ -760,7 +760,7 @@
       <c r="B5" s="2"/>
       <c r="C5" s="6"/>
       <c r="D5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E5" s="2"/>
     </row>
@@ -769,7 +769,7 @@
       <c r="B6" s="2"/>
       <c r="C6" s="6"/>
       <c r="D6" s="2" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E6" s="2"/>
     </row>
@@ -778,7 +778,7 @@
       <c r="B7" s="4"/>
       <c r="C7" s="7"/>
       <c r="D7" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E7" s="3"/>
     </row>
@@ -807,19 +807,19 @@
         <v>3</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="E9" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="F9" s="9" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -828,10 +828,10 @@
       <c r="C10" s="12"/>
       <c r="D10" s="12"/>
       <c r="E10" s="2" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -840,7 +840,7 @@
       <c r="C11" s="12"/>
       <c r="D11" s="12"/>
       <c r="E11" s="2" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F11" s="9"/>
     </row>

</xml_diff>